<commit_message>
update version 0.2.1, No es version nueva, solo actualizacion
</commit_message>
<xml_diff>
--- a/fhir/ig/tei/0.2.1/StructureDefinition-AllergyIntoleranceIniciarLE.xlsx
+++ b/fhir/ig/tei/0.2.1/StructureDefinition-AllergyIntoleranceIniciarLE.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="410">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-25T17:22:41-04:00</t>
+    <t>2024-07-15T11:25:06-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -501,7 +501,7 @@
     <t>active | inactive | resolved</t>
   </si>
   <si>
-    <t>The clinical status of the allergy or intolerance.</t>
+    <t>Estado clínico de la alergía o la intolerancia</t>
   </si>
   <si>
     <t>Refer to [discussion](http://hl7.org/fhir/R4/extensibility.html#Special-Case) if clincalStatus is missing data.
@@ -511,6 +511,9 @@
     <t>required</t>
   </si>
   <si>
+    <t>The clinical status of the allergy or intolerance.</t>
+  </si>
+  <si>
     <t>http://hl7.org/fhir/ValueSet/allergyintolerance-clinical|4.0.1</t>
   </si>
   <si>
@@ -530,7 +533,7 @@
     <t>unconfirmed | confirmed | refuted | entered-in-error</t>
   </si>
   <si>
-    <t>Assertion about certainty associated with the propensity, or potential risk, of a reaction to the identified substance (including pharmaceutical product).</t>
+    <t>Estado de verificación de la alergía o la intolerancia</t>
   </si>
   <si>
     <t>The data type is CodeableConcept because verificationStatus has some clinical judgment involved, such that there might need to be more specificity than the required FHIR value set allows. For example, a SNOMED coding might allow for additional specificity.</t>
@@ -2923,7 +2926,7 @@
         <v>86</v>
       </c>
       <c r="H12" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="I12" t="s" s="2">
         <v>87</v>
@@ -2970,10 +2973,10 @@
         <v>157</v>
       </c>
       <c r="Y12" t="s" s="2">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="Z12" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="AA12" t="s" s="2">
         <v>78</v>
@@ -3000,16 +3003,16 @@
         <v>86</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="AJ12" t="s" s="2">
         <v>98</v>
       </c>
       <c r="AK12" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AL12" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AM12" t="s" s="2">
         <v>78</v>
@@ -3017,10 +3020,10 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" t="s" s="2">
@@ -3034,7 +3037,7 @@
         <v>86</v>
       </c>
       <c r="H13" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="I13" t="s" s="2">
         <v>87</v>
@@ -3046,13 +3049,13 @@
         <v>153</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="N13" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="O13" s="2"/>
       <c r="P13" t="s" s="2">
@@ -3081,10 +3084,10 @@
         <v>157</v>
       </c>
       <c r="Y13" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Z13" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="AA13" t="s" s="2">
         <v>78</v>
@@ -3102,7 +3105,7 @@
         <v>78</v>
       </c>
       <c r="AF13" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AG13" t="s" s="2">
         <v>76</v>
@@ -3111,16 +3114,16 @@
         <v>86</v>
       </c>
       <c r="AI13" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="AJ13" t="s" s="2">
         <v>98</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AM13" t="s" s="2">
         <v>78</v>
@@ -3128,14 +3131,14 @@
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" t="s" s="2">
@@ -3157,13 +3160,13 @@
         <v>106</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="N14" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="O14" s="2"/>
       <c r="P14" t="s" s="2">
@@ -3192,10 +3195,10 @@
         <v>157</v>
       </c>
       <c r="Y14" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="Z14" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AA14" t="s" s="2">
         <v>78</v>
@@ -3213,7 +3216,7 @@
         <v>78</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AG14" t="s" s="2">
         <v>76</v>
@@ -3228,25 +3231,25 @@
         <v>98</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="AL14" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="AM14" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" t="s" s="2">
@@ -3268,13 +3271,13 @@
         <v>106</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N15" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="O15" s="2"/>
       <c r="P15" t="s" s="2">
@@ -3303,10 +3306,10 @@
         <v>157</v>
       </c>
       <c r="Y15" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="Z15" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AA15" t="s" s="2">
         <v>78</v>
@@ -3324,7 +3327,7 @@
         <v>78</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="AG15" t="s" s="2">
         <v>76</v>
@@ -3339,25 +3342,25 @@
         <v>98</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="AM15" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" t="s" s="2">
@@ -3379,13 +3382,13 @@
         <v>106</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="N16" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="O16" s="2"/>
       <c r="P16" t="s" s="2">
@@ -3414,10 +3417,10 @@
         <v>157</v>
       </c>
       <c r="Y16" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="Z16" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="AA16" t="s" s="2">
         <v>78</v>
@@ -3435,7 +3438,7 @@
         <v>78</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AG16" t="s" s="2">
         <v>76</v>
@@ -3450,25 +3453,25 @@
         <v>98</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" t="s" s="2">
@@ -3490,13 +3493,13 @@
         <v>153</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="N17" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="O17" s="2"/>
       <c r="P17" t="s" s="2">
@@ -3526,7 +3529,7 @@
       </c>
       <c r="Y17" s="2"/>
       <c r="Z17" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AA17" t="s" s="2">
         <v>78</v>
@@ -3544,7 +3547,7 @@
         <v>78</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>76</v>
@@ -3559,21 +3562,21 @@
         <v>98</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
@@ -3596,13 +3599,13 @@
         <v>78</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
@@ -3653,7 +3656,7 @@
         <v>78</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>76</v>
@@ -3668,7 +3671,7 @@
         <v>78</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="AL18" t="s" s="2">
         <v>78</v>
@@ -3679,10 +3682,10 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
@@ -3711,7 +3714,7 @@
         <v>133</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="N19" t="s" s="2">
         <v>135</v>
@@ -3752,19 +3755,19 @@
         <v>78</v>
       </c>
       <c r="AB19" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="AC19" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="AD19" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>76</v>
@@ -3779,7 +3782,7 @@
         <v>137</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="AL19" t="s" s="2">
         <v>78</v>
@@ -3790,10 +3793,10 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
@@ -3816,19 +3819,19 @@
         <v>87</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="N20" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="O20" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="P20" t="s" s="2">
         <v>78</v>
@@ -3877,7 +3880,7 @@
         <v>78</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>76</v>
@@ -3892,21 +3895,21 @@
         <v>98</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AL20" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
@@ -3929,13 +3932,13 @@
         <v>78</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
@@ -3986,7 +3989,7 @@
         <v>78</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>76</v>
@@ -4001,7 +4004,7 @@
         <v>78</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="AL21" t="s" s="2">
         <v>78</v>
@@ -4012,10 +4015,10 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -4044,7 +4047,7 @@
         <v>133</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="N22" t="s" s="2">
         <v>135</v>
@@ -4085,19 +4088,19 @@
         <v>78</v>
       </c>
       <c r="AB22" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="AC22" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="AD22" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>76</v>
@@ -4112,7 +4115,7 @@
         <v>137</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="AL22" t="s" s="2">
         <v>78</v>
@@ -4123,10 +4126,10 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -4152,16 +4155,16 @@
         <v>100</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="N23" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="O23" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="P23" t="s" s="2">
         <v>78</v>
@@ -4210,7 +4213,7 @@
         <v>78</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>76</v>
@@ -4225,21 +4228,21 @@
         <v>98</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="AL23" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -4262,16 +4265,16 @@
         <v>87</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="O24" s="2"/>
       <c r="P24" t="s" s="2">
@@ -4321,7 +4324,7 @@
         <v>78</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>76</v>
@@ -4336,21 +4339,21 @@
         <v>98</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AL24" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
@@ -4376,14 +4379,14 @@
         <v>106</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="P25" t="s" s="2">
         <v>78</v>
@@ -4432,7 +4435,7 @@
         <v>78</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>76</v>
@@ -4447,21 +4450,21 @@
         <v>98</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AL25" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -4484,17 +4487,17 @@
         <v>87</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="P26" t="s" s="2">
         <v>78</v>
@@ -4543,7 +4546,7 @@
         <v>78</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>76</v>
@@ -4558,21 +4561,21 @@
         <v>98</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AL26" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -4595,19 +4598,19 @@
         <v>87</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="O27" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="P27" t="s" s="2">
         <v>78</v>
@@ -4656,7 +4659,7 @@
         <v>78</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>76</v>
@@ -4671,21 +4674,21 @@
         <v>98</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="AL27" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -4708,19 +4711,19 @@
         <v>87</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="O28" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="P28" t="s" s="2">
         <v>78</v>
@@ -4769,7 +4772,7 @@
         <v>78</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>76</v>
@@ -4784,25 +4787,25 @@
         <v>98</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AL28" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" t="s" s="2">
@@ -4821,13 +4824,13 @@
         <v>87</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -4878,7 +4881,7 @@
         <v>78</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>86</v>
@@ -4893,21 +4896,21 @@
         <v>98</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -4930,13 +4933,13 @@
         <v>78</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
@@ -4987,7 +4990,7 @@
         <v>78</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>76</v>
@@ -5002,7 +5005,7 @@
         <v>78</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="AL30" t="s" s="2">
         <v>78</v>
@@ -5013,10 +5016,10 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5045,7 +5048,7 @@
         <v>133</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="N31" t="s" s="2">
         <v>135</v>
@@ -5086,19 +5089,19 @@
         <v>78</v>
       </c>
       <c r="AB31" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="AC31" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="AD31" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>76</v>
@@ -5113,7 +5116,7 @@
         <v>137</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="AL31" t="s" s="2">
         <v>78</v>
@@ -5124,10 +5127,10 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5150,16 +5153,16 @@
         <v>87</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="N32" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="O32" s="2"/>
       <c r="P32" t="s" s="2">
@@ -5209,7 +5212,7 @@
         <v>78</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>76</v>
@@ -5218,7 +5221,7 @@
         <v>86</v>
       </c>
       <c r="AI32" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="AJ32" t="s" s="2">
         <v>98</v>
@@ -5235,10 +5238,10 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5264,13 +5267,13 @@
         <v>100</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="O33" s="2"/>
       <c r="P33" t="s" s="2">
@@ -5296,13 +5299,13 @@
         <v>78</v>
       </c>
       <c r="X33" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="Y33" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="Z33" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="AA33" t="s" s="2">
         <v>78</v>
@@ -5320,7 +5323,7 @@
         <v>78</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>76</v>
@@ -5346,10 +5349,10 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5375,13 +5378,13 @@
         <v>144</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="N34" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="O34" s="2"/>
       <c r="P34" t="s" s="2">
@@ -5431,7 +5434,7 @@
         <v>78</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>76</v>
@@ -5446,7 +5449,7 @@
         <v>98</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="AL34" t="s" s="2">
         <v>78</v>
@@ -5457,10 +5460,10 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -5483,16 +5486,16 @@
         <v>87</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="N35" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="O35" s="2"/>
       <c r="P35" t="s" s="2">
@@ -5542,7 +5545,7 @@
         <v>78</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>76</v>
@@ -5568,10 +5571,10 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -5594,13 +5597,13 @@
         <v>78</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
@@ -5651,7 +5654,7 @@
         <v>78</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>76</v>
@@ -5666,10 +5669,10 @@
         <v>98</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="AM36" t="s" s="2">
         <v>78</v>
@@ -5677,10 +5680,10 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -5703,13 +5706,13 @@
         <v>78</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
@@ -5760,7 +5763,7 @@
         <v>78</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>76</v>
@@ -5775,10 +5778,10 @@
         <v>98</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AM37" t="s" s="2">
         <v>78</v>
@@ -5786,10 +5789,10 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -5812,13 +5815,13 @@
         <v>78</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
@@ -5869,7 +5872,7 @@
         <v>78</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>76</v>
@@ -5884,25 +5887,25 @@
         <v>98</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" t="s" s="2">
@@ -5921,13 +5924,13 @@
         <v>78</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -5978,7 +5981,7 @@
         <v>78</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>76</v>
@@ -5993,10 +5996,10 @@
         <v>98</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="AM39" t="s" s="2">
         <v>78</v>
@@ -6004,14 +6007,14 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" t="s" s="2">
@@ -6030,16 +6033,16 @@
         <v>87</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="O40" s="2"/>
       <c r="P40" t="s" s="2">
@@ -6089,7 +6092,7 @@
         <v>78</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>76</v>
@@ -6104,21 +6107,21 @@
         <v>98</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6141,16 +6144,16 @@
         <v>78</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="O41" s="2"/>
       <c r="P41" t="s" s="2">
@@ -6200,7 +6203,7 @@
         <v>78</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>76</v>
@@ -6215,7 +6218,7 @@
         <v>98</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="AL41" t="s" s="2">
         <v>78</v>
@@ -6226,10 +6229,10 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6252,16 +6255,16 @@
         <v>78</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="O42" s="2"/>
       <c r="P42" t="s" s="2">
@@ -6311,7 +6314,7 @@
         <v>78</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>76</v>
@@ -6326,7 +6329,7 @@
         <v>98</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="AL42" t="s" s="2">
         <v>78</v>
@@ -6337,10 +6340,10 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6363,13 +6366,13 @@
         <v>78</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
@@ -6420,7 +6423,7 @@
         <v>78</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>76</v>
@@ -6435,7 +6438,7 @@
         <v>98</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="AL43" t="s" s="2">
         <v>78</v>
@@ -6446,10 +6449,10 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -6472,13 +6475,13 @@
         <v>78</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
@@ -6529,7 +6532,7 @@
         <v>78</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>76</v>
@@ -6544,7 +6547,7 @@
         <v>78</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="AL44" t="s" s="2">
         <v>78</v>
@@ -6555,10 +6558,10 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -6587,7 +6590,7 @@
         <v>133</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="N45" t="s" s="2">
         <v>135</v>
@@ -6640,7 +6643,7 @@
         <v>78</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>76</v>
@@ -6655,7 +6658,7 @@
         <v>137</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="AL45" t="s" s="2">
         <v>78</v>
@@ -6666,14 +6669,14 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" t="s" s="2">
@@ -6695,10 +6698,10 @@
         <v>132</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="N46" t="s" s="2">
         <v>135</v>
@@ -6753,7 +6756,7 @@
         <v>78</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>76</v>
@@ -6779,10 +6782,10 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -6808,13 +6811,13 @@
         <v>153</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="O47" s="2"/>
       <c r="P47" t="s" s="2">
@@ -6840,13 +6843,13 @@
         <v>78</v>
       </c>
       <c r="X47" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="Y47" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="Z47" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="AA47" t="s" s="2">
         <v>78</v>
@@ -6864,7 +6867,7 @@
         <v>78</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>76</v>
@@ -6879,7 +6882,7 @@
         <v>98</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="AL47" t="s" s="2">
         <v>78</v>
@@ -6890,14 +6893,14 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" t="s" s="2">
@@ -6919,13 +6922,13 @@
         <v>153</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="O48" s="2"/>
       <c r="P48" t="s" s="2">
@@ -6951,13 +6954,13 @@
         <v>78</v>
       </c>
       <c r="X48" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="Y48" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="Z48" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="AA48" t="s" s="2">
         <v>78</v>
@@ -6975,7 +6978,7 @@
         <v>78</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>86</v>
@@ -6990,25 +6993,25 @@
         <v>98</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="AL48" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" t="s" s="2">
@@ -7027,16 +7030,16 @@
         <v>78</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="O49" s="2"/>
       <c r="P49" t="s" s="2">
@@ -7086,7 +7089,7 @@
         <v>78</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>76</v>
@@ -7101,7 +7104,7 @@
         <v>98</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="AL49" t="s" s="2">
         <v>78</v>
@@ -7112,10 +7115,10 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -7138,13 +7141,13 @@
         <v>78</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
@@ -7195,7 +7198,7 @@
         <v>78</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>76</v>
@@ -7210,21 +7213,21 @@
         <v>98</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="AL50" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -7250,13 +7253,13 @@
         <v>106</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="O51" s="2"/>
       <c r="P51" t="s" s="2">
@@ -7285,10 +7288,10 @@
         <v>157</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="Z51" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="AA51" t="s" s="2">
         <v>78</v>
@@ -7306,7 +7309,7 @@
         <v>78</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>76</v>
@@ -7321,7 +7324,7 @@
         <v>98</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="AL51" t="s" s="2">
         <v>78</v>
@@ -7332,10 +7335,10 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -7361,13 +7364,13 @@
         <v>153</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="O52" s="2"/>
       <c r="P52" t="s" s="2">
@@ -7393,13 +7396,13 @@
         <v>78</v>
       </c>
       <c r="X52" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="Y52" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="Z52" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="AA52" t="s" s="2">
         <v>78</v>
@@ -7417,7 +7420,7 @@
         <v>78</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>76</v>
@@ -7432,7 +7435,7 @@
         <v>98</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AL52" t="s" s="2">
         <v>78</v>
@@ -7443,10 +7446,10 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -7469,16 +7472,16 @@
         <v>78</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="N53" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="O53" s="2"/>
       <c r="P53" t="s" s="2">
@@ -7528,7 +7531,7 @@
         <v>78</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>76</v>
@@ -7543,7 +7546,7 @@
         <v>98</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="AL53" t="s" s="2">
         <v>78</v>

</xml_diff>